<commit_message>
first pass of the crossword object working well - allows placement including validation
</commit_message>
<xml_diff>
--- a/data/puzzle_samples/mini_03262025.xlsx
+++ b/data/puzzle_samples/mini_03262025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\witzi\OneDrive\Documents\neu_part_2\CS5100_FAI\code\ai_crossword_solver\data\puzzle_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11FC737-DC22-4CAA-8F71-5C7C95B48CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA05D87C-6312-4F38-A980-6666C7CE2B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="23700" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>number</t>
   </si>
@@ -84,6 +84,42 @@
   </si>
   <si>
     <t>end_row</t>
+  </si>
+  <si>
+    <t>answer (optional column, for checking only)</t>
+  </si>
+  <si>
+    <t>length (optional column, for checking only)</t>
+  </si>
+  <si>
+    <t>tab</t>
+  </si>
+  <si>
+    <t>irl</t>
+  </si>
+  <si>
+    <t>paris</t>
+  </si>
+  <si>
+    <t>broth</t>
+  </si>
+  <si>
+    <t>jazzy</t>
+  </si>
+  <si>
+    <t>tiara</t>
+  </si>
+  <si>
+    <t>arroz</t>
+  </si>
+  <si>
+    <t>blitz</t>
+  </si>
+  <si>
+    <t>pbj</t>
+  </si>
+  <si>
+    <t>shy</t>
   </si>
 </sst>
 </file>
@@ -407,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -420,11 +456,13 @@
     <col min="3" max="3" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="55.6640625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="30.21875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="36.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,8 +481,14 @@
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -463,8 +507,14 @@
       <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>4</v>
       </c>
@@ -483,8 +533,14 @@
       <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>5</v>
       </c>
@@ -503,8 +559,14 @@
       <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>7</v>
       </c>
@@ -523,8 +585,14 @@
       <c r="F5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>8</v>
       </c>
@@ -543,8 +611,14 @@
       <c r="F6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -563,8 +637,14 @@
       <c r="F7" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -583,8 +663,14 @@
       <c r="F8" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -603,8 +689,14 @@
       <c r="F9" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -623,8 +715,14 @@
       <c r="F10" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>6</v>
       </c>
@@ -642,6 +740,12 @@
       </c>
       <c r="F11" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>